<commit_message>
Played with a brace counting approach
</commit_message>
<xml_diff>
--- a/CH-164 Extract from Text.xlsx
+++ b/CH-164 Extract from Text.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E48678F-FBB9-4370-8F5A-A9D94F7E3F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCC9AFD-D05C-45F0-AF7B-3EC63530AA03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="5" r:id="rId4"/>
+    <sheet name="Alt3" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_fBCAST">_xlfn.LAMBDA(_xlpm._nData, _xlfn.LET(_xlpm.f, _xlfn.LAMBDA(_xlpm._d, _xlfn.LET(_xlpm._c, COLUMNS(_xlpm._d) - 1, _xlfn.DROP(_xlfn.REDUCE("", _xlfn.TAKE(_xlpm._d, , 1), _xlfn.LAMBDA(_xlpm.a,_xlpm.v, _xlfn.VSTACK(_xlpm.a, _xlfn.EXPAND(_xlpm.v, _xlpm._c, 1, _xlpm.v)))), 1))), _xlfn.HSTACK(_xlpm.f(_xlpm._nData), _xlfn.TOCOL(_xlfn.DROP(_xlpm._nData, , 1)))))</definedName>
+    <definedName name="_fCharCount">_xlfn.LAMBDA(_xlpm.s,_xlpm.c, _xlfn.LET(_xlpm.z, SUBSTITUTE(_xlpm.s, _xlpm.c, ""), LEN(_xlpm.s) - LEN(_xlpm.z)))</definedName>
+    <definedName name="_fDN">_xlfn.LAMBDA(_xlpm.arr,_xlop.ini, _xlfn.LET(_xlpm._ini, IF(_xlfn.ISOMITTED(_xlpm.ini), "", _xlpm.ini), _xlfn.SCAN(_xlpm._ini, _xlpm.arr, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, IF(LEN(_xlpm.v) = 0, _xlpm.a, _xlpm.v)))))</definedName>
+    <definedName name="_fDX">_xlfn.LAMBDA(_xlpm.vlookup_value,_xlpm.vlookup_array,_xlpm.hlookup_value,_xlpm.hlookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.vmatch_mode,_xlop.vsearch_mode,_xlop.hmatch_mode,_xlop.hsearch_mode, IFERROR(INDEX(_xlpm.return_array, _xlfn.XMATCH(_xlpm.vlookup_value, _xlpm.vlookup_array, _xlpm.vmatch_mode, _xlpm.vsearch_mode), _xlfn.XMATCH(_xlpm.hlookup_value, _xlpm.hlookup_array, _xlpm.hmatch_mode, _xlpm.hsearch_mode)), IF(ISOMlTTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)))</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt3'!$B$2:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$C$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$C$7</definedName>
+    <definedName name="_fIndex">_xlfn.LAMBDA(_xlpm.d,_xlpm.r, INDEX(_xlpm.d, _xlpm.r, _xlfn.SEQUENCE(1, COLUMNS(_xlpm.d))))</definedName>
+    <definedName name="_fInterp">_xlfn.LAMBDA(_xlpm.x,_xlpm.xdat,_xlpm.ydat, _xlfn.LET(_xlpm.xmin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , -1), _xlpm.xmax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.xdat, , 1), _xlpm.ymin, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , -1), _xlpm.ymax, _xlfn.XLOOKUP(_xlpm.x, _xlpm.xdat, _xlpm.ydat, , 1), IF(_xlpm.xmin = _xlpm.xmax, _xlpm.ymin, (_xlpm.ymin * (_xlpm.xmax - _xlpm.x) + _xlpm.ymax * (_xlpm.x - _xlpm.xmin)) / (_xlpm.xmax - _xlpm.xmin))))</definedName>
+    <definedName name="_fQ">_xlfn.LAMBDA(_xlpm.x, ROUNDUP(MONTH(1 &amp; _xlpm.x) / 3, 0))</definedName>
+    <definedName name="_fSUPERXLOOKUP">_xlfn.LAMBDA(_xlpm.lookup_value,_xlpm.lookup_array,_xlpm.return_array,_xlop.if_not_found,_xlop.match_mode,_xlop.search_mode, IF(COLUMNS(_xlpm.lookup_value) = 1, IFERROR(INDEX(_xlpm.return_array, _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode), _xlfn.SEQUENCE(1, COLUMNS(_xlpm.return_array))), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found)), IFERROR(INDEX(_xlpm.return_array, _xlfn.SEQUENCE(ROWS(_xlpm.return_array)), _xlfn.XMATCH(_xlpm.lookup_value, _xlpm.lookup_array, _xlpm.match_mode, _xlpm.search_mode)), IF(_xlfn.ISOMITTED(_xlpm.if_not_found), NA(), _xlpm.if_not_found))))</definedName>
+    <definedName name="_fUP">_xlfn.LAMBDA(_xlpm.arr,_xlop.ini, _xlfn.LET(_xlpm._f, _xlfn.LAMBDA(_xlpm.z, INDEX(_xlpm.z, _xlfn.SEQUENCE(ROWS(_xlpm.z), 1, ROWS(_xlpm.z), -1))), _xlpm._arr, _xlpm._f(_xlpm.arr), _xlpm._ini, IF(_xlfn.ISOMITTED(_xlpm.ini), "", _xlpm.ini), _xlpm._f(_xlfn.SCAN(_xlpm._ini, _xlpm._arr, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, IF(LEN(_xlpm.v) = 0, _xlpm.a, _xlpm.v))))))</definedName>
+    <definedName name="DDL">_xlfn.LAMBDA(_xlpm.range,_xlop.lookup1,_xlop.lookup2,_xlop.lookup3,_xlop.lookup4,_xlop.lookup5,_xlop.lookup6,_xlop.lookup7,_xlop.lookup8,_xlop.lookup9,_xlop.lookup10, _xlfn.LET(_xlpm._s, "%^&amp;&amp;@", _xlpm.lookupValue, _xlpm.lookup1 &amp; _xlpm._s &amp; _xlpm.lookup2 &amp; _xlpm._s &amp; _xlpm.lookup3 &amp; _xlpm._s &amp; _xlpm.lookup4 &amp; _xlpm._s &amp; _xlpm.lookup5 &amp; _xlpm._s &amp; _xlpm.lookup6 &amp; _xlpm._s &amp; _xlpm.lookup7 &amp; _xlpm._s &amp; _xlpm.lookup8 &amp; _xlpm._s &amp; _xlpm.lookup9 &amp; _xlpm._s &amp; _xlpm.lookup10, _xlpm.levelIndex, IFERROR(ROWS(_xlfn.TEXTSPLIT(_xlpm.lookupValue, , _xlpm._s, TRUE())), 0) + 1, _xlpm.lookupArray, _xlfn.BYROW(_xlfn.EXPAND(_xlfn.CHOOSECOLS(_xlpm.range, _xlfn.SEQUENCE(1, _xlpm.levelIndex - 1)), , 10, ""), _xlfn.LAMBDA(_xlpm.row, _xlfn.TEXTJOIN(_xlpm._s, FALSE, _xlpm.row))), _xlpm.returnRange, INDEX(_xlpm.range, 0, _xlpm.levelIndex), _xlpm.result, IF(_xlfn.ISOMITTED(_xlpm.lookup1) * _xlpm.levelIndex = 1, _xlpm.returnRange, _xlfn.XLOOKUP(_xlpm.lookupValue, _xlpm.lookupArray, _xlpm.returnRange):_xlfn.XLOOKUP(_xlpm.lookupValue, _xlpm.lookupArray, _xlpm.returnRange, , , -1)), _xlpm.result))</definedName>
+    <definedName name="DDLSorter">_xlfn.LAMBDA(_xlpm.Range,_xlop.SortOrder, _xlfn._xlws.SORT(_xlpm.Range, _xlfn.SEQUENCE(, COLUMNS(_xlpm.Range)), _xlpm.SortOrder))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -232,6 +245,15 @@
   </si>
   <si>
     <t>This is a very clever non-regex solution. It only supports finding up to 3 levels.I am not sure it is bulletproof. I would need to think it through.</t>
+  </si>
+  <si>
+    <t>I like this approach the best. It scales and makes good use of a simple regex.</t>
+  </si>
+  <si>
+    <t>Interesting way to determine the number of characters in string.</t>
+  </si>
+  <si>
+    <t>I still don't know if I trust this as bulletproof</t>
   </si>
 </sst>
 </file>
@@ -438,9 +460,6 @@
     <xf numFmtId="1" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -449,6 +468,9 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,7 +1063,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="567" row="9">
+  <wetp:taskpane dockstate="right" visibility="0" width="307" row="9">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1053,10 +1075,15 @@
   <we:alternateReferences>
     <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
   </we:alternateReferences>
-  <we:properties/>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{5714F15D-BBBC-4CEE-B2FC-197F7FBAB617}&quot;}"/>
+  </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1071,7 +1098,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1085,14 +1112,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="E1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="15"/>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="E1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="18"/>
       <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
@@ -1284,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40350A12-9488-4088-A0F3-CC16B5B8F397}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1299,14 +1326,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="E1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="15"/>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="E1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="18"/>
       <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
@@ -1417,7 +1444,7 @@
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B10" s="4"/>
-      <c r="C10" s="16" t="str" cm="1">
+      <c r="C10" s="15" t="str" cm="1">
         <f t="array" ref="C10:C18">MID(C4,_xlfn.SEQUENCE(LEN(C3)),1)</f>
         <v>{</v>
       </c>
@@ -1543,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE1BA0B-D7CC-40F2-B60F-F698508D3F97}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1558,14 +1585,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="E1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="15"/>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="E1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="18"/>
       <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
@@ -1673,6 +1700,9 @@
       <c r="D9" s="9"/>
       <c r="E9"/>
       <c r="F9"/>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B10" s="4"/>
@@ -1696,7 +1726,7 @@
     </row>
     <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B12" s="4"/>
-      <c r="C12" s="17" cm="1">
+      <c r="C12" s="16" cm="1">
         <f t="array" ref="C12:C16">_xlfn.MAP(
     C3:C7,
     _xlfn.LAMBDA(_xlpm.a,
@@ -1829,7 +1859,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" s="1"/>
       <c r="D18" s="10"/>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="17" t="s">
         <v>9</v>
       </c>
       <c r="F18">
@@ -1840,7 +1870,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19" s="1"/>
       <c r="D19" s="10"/>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="17" t="s">
         <v>5</v>
       </c>
       <c r="F19">
@@ -1850,7 +1880,7 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F20">
@@ -1860,7 +1890,7 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F21">
@@ -1870,7 +1900,7 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F22">
@@ -1894,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBA7083-87AC-43DD-870A-917E5890301E}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
@@ -1909,14 +1939,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="E1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="15"/>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="E1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="18"/>
       <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
@@ -2128,4 +2158,495 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703E0068-8383-466F-80F4-ACFCCF8B4D84}">
+  <dimension ref="A1:V23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.21875" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="E1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="J1" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="12">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="12">
+        <v>3</v>
+      </c>
+      <c r="F5" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="12">
+        <v>4</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>5</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="12">
+        <v>5</v>
+      </c>
+      <c r="F7" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="9"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="4"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="4"/>
+      <c r="C10" cm="1">
+        <f t="array" ref="C10:C14">_xlfn.BYROW(
+    C3:C7 = SUBSTITUTE(C3:C7, REPT("}", _xlfn.SEQUENCE(, 5)), ""),
+    _xlfn.LAMBDA(_xlpm.A, _xlfn.XMATCH(1, --_xlpm.A))
+) - 2</f>
+        <v>1</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10" t="b" cm="1">
+        <f t="array" ref="G10:K14">C3:C7 = SUBSTITUTE(C3:C7, REPT("}", _xlfn.SEQUENCE(, 5)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10" cm="1">
+        <f t="array" ref="M10">_xlfn.XMATCH(1,--G10:K10)</f>
+        <v>3</v>
+      </c>
+      <c r="N10" s="2">
+        <f>M10-2</f>
+        <v>1</v>
+      </c>
+      <c r="P10" s="2" cm="1">
+        <f t="array" ref="P10:T10">_fCharCount(C3,REPT("}", _xlfn.SEQUENCE(, 5)))</f>
+        <v>2</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>2</v>
+      </c>
+      <c r="R10" s="2">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2">
+        <f>MAX(_xlfn.ANCHORARRAY(P10))-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="4"/>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11"/>
+      <c r="M11" cm="1">
+        <f t="array" ref="M11">_xlfn.XMATCH(1,--G11:K11)</f>
+        <v>3</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" ref="N11:N14" si="0">M11-2</f>
+        <v>1</v>
+      </c>
+      <c r="P11" s="2" cm="1">
+        <f t="array" ref="P11:T11">_fCharCount(C4,REPT("}", _xlfn.SEQUENCE(, 5)))</f>
+        <v>2</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>2</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <f>MAX(_xlfn.ANCHORARRAY(P11))-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="4"/>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12" cm="1">
+        <f t="array" ref="M12">_xlfn.XMATCH(1,--G12:K12)</f>
+        <v>3</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P12" s="2" cm="1">
+        <f t="array" ref="P12:T12">_fCharCount(C5,REPT("}", _xlfn.SEQUENCE(, 5)))</f>
+        <v>3</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>2</v>
+      </c>
+      <c r="R12" s="2">
+        <v>0</v>
+      </c>
+      <c r="S12" s="2">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2">
+        <f>MAX(_xlfn.ANCHORARRAY(P12))-1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="E13"/>
+      <c r="G13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" cm="1">
+        <f t="array" ref="M13">_xlfn.XMATCH(1,--G13:K13)</f>
+        <v>2</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="2" cm="1">
+        <f t="array" ref="P13:T13">_fCharCount(C6,REPT("}", _xlfn.SEQUENCE(, 5)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="V13" s="2">
+        <f>MAX(_xlfn.ANCHORARRAY(P13))-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14"/>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" cm="1">
+        <f t="array" ref="M14">_xlfn.XMATCH(1,--G14:K14)</f>
+        <v>4</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P14" s="2" cm="1">
+        <f t="array" ref="P14:T14">_fCharCount(C7,REPT("}", _xlfn.SEQUENCE(, 5)))</f>
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>3</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="V14" s="2">
+        <f>MAX(_xlfn.ANCHORARRAY(P14))-1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A15" s="1"/>
+      <c r="C15"/>
+      <c r="E15"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.5">
+      <c r="A16" s="1"/>
+      <c r="C16"/>
+      <c r="E16"/>
+      <c r="P16" cm="1">
+        <f t="array" ref="P16:P20">_xlfn.DROP(_xlfn.REDUCE("",C3:C7,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,MAX(_fCharCount(_xlpm.v,REPT("}", _xlfn.SEQUENCE(, 5))))))),1)-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A17" s="1"/>
+      <c r="C17"/>
+      <c r="E17"/>
+      <c r="P17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A18" s="1"/>
+      <c r="C18"/>
+      <c r="E18"/>
+      <c r="P18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A19" s="1"/>
+      <c r="C19"/>
+      <c r="E19"/>
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A20" s="1"/>
+      <c r="C20"/>
+      <c r="E20"/>
+      <c r="P20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A21" s="1"/>
+      <c r="C21"/>
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A22" s="1"/>
+      <c r="C22"/>
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="D23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AXABuAC8ALwAgAEcAZQBuAGUAcgBhAHQAZQAgAGEAbgAgAGkAbgBkAGUAeAAgAGMAbwBsAHUAbQBuACAAdABoAGUAIABoAGUAaQBnAGgAdAAgAG8AZgAgAHQAaABlACAAZABhAHQAYQAgAGQAXABuAF8AZgBJAG4AZABlAHgAPQBMAEEATQBCAEQAQQAoAGQALAByACwASQBOAEQARQBYACgAZAAsAHIALABTAEUAUQBVAEUATgBDAEUAKAAxACwAQwBPAEwAVQBNAE4AUwAoAGQAKQApACkAKQA7AFwAbgAvAC8AIABTAHUAcABlAHIAWABMAE8ATwBLAFUAUABcAG4AXwBmAFMAVQBQAEUAUgBYAEwATwBPAEsAVQBQAD0ATABBAE0AQgBEAEEAKABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsAGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABbAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkAF0ALABbAG0AYQB0AGMAaABfAG0AbwBkAGUAXQAsAFsAcwBlAGEAcgBjAGgAXwBtAG8AZABlAF0ALABcAG4AIAAgACAAIABJAEYAKABcAG4AIAAgACAAIAAgACAAIAAgAEMATwBMAFUATQBOAFMAKABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQApACAAPQAgADEALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgBFAFIAUgBPAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABYAE0AQQBUAEMASAAoAGwAbwBvAGsAdQBwAF8AdgBhAGwAdQBlACwAIABsAG8AbwBrAHUAcABfAGEAcgByAGEAeQAsACAAbQBhAHQAYwBoAF8AbQBvAGQAZQAsACAAcwBlAGEAcgBjAGgAXwBtAG8AZABlACkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKAAxACwAIABDAE8ATABVAE0ATgBTACgAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkAKQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQAsACAATgBBACgAKQAsACAAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACkALABcAG4AIAAgACAAIAAgACAAIAAgAEkARgBFAFIAUgBPAFIAKABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAASQBOAEQARQBYACgAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABcAG4AIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIABTAEUAUQBVAEUATgBDAEUAKABSAE8AVwBTACgAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkAKQApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAWABNAEEAVABDAEgAKABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsACAAbABvAG8AawB1AHAAXwBhAHIAcgBhAHkALAAgAG0AYQB0AGMAaABfAG0AbwBkAGUALAAgAHMAZQBhAHIAYwBoAF8AbQBvAGQAZQApAFwAbgAgACAAIAAgACAAIAAgACAAIAAgACAAIAApACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgAEkARgAoAEkAUwBPAE0ASQBUAFQARQBEACgAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQAsACAATgBBACgAKQAsACAAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQBcAG4AIAAgACAAIAAgACAAIAAgACkAXABuACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAvACAATABpAG4AZQBhAHIAIABJAG4AdABlAHIAcABvAGwAYQB0AGkAbwBuACAARgBvAHIAbQB1AGwAYQBcAG4AXwBmAEkAbgB0AGUAcgBwAD0ATABBAE0AQgBEAEEAKAB4ACwAeABkAGEAdAAsAHkAZABhAHQALABcAG4AIAAgACAAIAAgAEwARQBUACgAXABuACAAIAAgACAAIAAgACAAIAAgAHgAbQBpAG4ALAAgAFgATABPAE8ASwBVAFAAKAB4ACwAeABkAGEAdAAsAHgAZABhAHQALAAsAC0AMQApACwAXABuACAAIAAgACAAIAAgACAAIAAgAHgAbQBhAHgALAAgAFgATABPAE8ASwBVAFAAKAB4ACwAeABkAGEAdAAsAHgAZABhAHQALAAsADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAB5AG0AaQBuACwAIABYAEwATwBPAEsAVQBQACgAeAAsAHgAZABhAHQALAB5AGQAYQB0ACwALAAtADEAKQAsAFwAbgAgACAAIAAgACAAIAAgACAAIAB5AG0AYQB4ACwAIABYAEwATwBPAEsAVQBQACgAeAAsAHgAZABhAHQALAB5AGQAYQB0ACwALAAxACkALABcAG4AIAAgACAAIAAgACAAIAAgACAASQBGACgAeABtAGkAbgA9AHgAbQBhAHgALAB5AG0AaQBuACwAXABuACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACAAIAAgACgAeQBtAGkAbgAqACgAeABtAGEAeAAtAHgAKQArAHkAbQBhAHgAKgAoAHgALQB4AG0AaQBuACkAKQAvACgAeABtAGEAeAAtAHgAbQBpAG4AKQApAFwAbgAgACAAIAAgACAAKQBcAG4AKQA7AFwAbgBcAG4ALwAvACAAQwBvAHUAbgB0ACAAYQAgAHMAcABlAGMAaQBmAGkAYwAgAGMAaABhAHIAYQBjAHQAZQByACAAaQBuACAAYQAgAHMAdAByAGkAbgBnAFwAbgBfAGYAQwBoAGEAcgBDAG8AdQBuAHQAPQBMAEEATQBCAEQAQQAoAHMALABjACwATABFAFQAKAB6ACwAUwBVAEIAUwBUAEkAVABVAFQARQAoAHMALABjACwAXAAiAFwAIgApACwATABFAE4AKABzACkALQBMAEUATgAoAHoAKQApACkAOwBcAG4AXABuAC8ALwAgAEYAaQBsAGwAIABEAG8AdwBuAFwAbgBfAGYARABOAD0ATABBAE0AQgBEAEEAKABhAHIAcgAsAFsAaQBuAGkAXQAsAFwAbgBMAEUAVAAoAFwAbgBfAGkAbgBpACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGkAbgBpACkALABcACIAXAAiACwAaQBuAGkAKQAsAFwAbgBTAEMAQQBOACgAXwBpAG4AaQAsAGEAcgByACwATABBAE0AQgBEAEEAKABhACwAdgAsAEkARgAoAEwARQBOACgAdgApAD0AMAAsAGEALAB2ACkAKQApAFwAbgApAFwAbgApADsAXABuAFwAbgAvAC8AIABGAGkAbABsACAAVQBwAFwAbgBfAGYAVQBQAD0ATABBAE0AQgBEAEEAKABhAHIAcgAsAFsAaQBuAGkAXQAsAFwAbgBMAEUAVAAoAFwAbgBfAGYALABMAEEATQBCAEQAQQAoAHoALABJAE4ARABFAFgAKAB6ACwAUwBFAFEAVQBFAE4AQwBFACgAUgBPAFcAUwAoAHoAKQAsADEALABSAE8AVwBTACgAegApACwALQAxACkAKQApACwAXABuAF8AYQByAHIALAAgAF8AZgAoAGEAcgByACkALABcAG4AXwBpAG4AaQAsACAASQBGACgASQBTAE8ATQBJAFQAVABFAEQAKABpAG4AaQApACwAXAAiAFwAIgAsAGkAbgBpACkALABcAG4AXwBmACgAUwBDAEEATgAoAF8AaQBuAGkALABfAGEAcgByACwATABBAE0AQgBEAEEAKABhACwAdgAsAEkARgAoAEwARQBOACgAdgApAD0AMAAsAGEALAB2ACkAKQApACkAXABuACkAXABuACkAOwBcAG4AXABuAC8ALwAgAEIAcgBvAGEAZABjAGEAcwB0ACAAZgBpAHIAcwB0ACAAYwBvAGwAdQBtAG4AXABuAF8AZgBCAEMAQQBTAFQAPQBMAEEATQBCAEQAQQAoAF8AbgBEAGEAdABhACwATABFAFQAKABmACwAIABMAEEATQBCAEQAQQAoAF8AZAAsAEwARQBUACgAXwBjACwAQwBPAEwAVQBNAE4AUwAoAF8AZAApAC0AMQAsAEQAUgBPAFAAKABSAEUARABVAEMARQAoAFwAIgBcACIALABUAEEASwBFACgAXwBkACwALAAxACkALABMAEEATQBCAEQAQQAoAGEALAB2ACwAVgBTAFQAQQBDAEsAKABhACwARQBYAFAAQQBOAEQAKAB2ACwAXwBjACwAMQAsAHYAKQApACkAKQAsADEAKQApACkALABcAG4AIAAgACAAIAAgAEgAUwBUAEEAQwBLACgAZgAoAF8AbgBEAGEAdABhACkALABUAE8AQwBPAEwAKABEAFIATwBQACgAXwBuAEQAYQB0AGEALAAsADEAKQApACkAXABuACkAKQA7AFwAbgBcAG4ALwAvACAATQBhAHIAawAgAFAAcgBvAGMAdABvAHIAIABEAEQATAAgAGYAdQBuAGMAdABpAG8AbgBcAG4ARABEAEwAPQBMAEEATQBCAEQAQQAoAHIAYQBuAGcAZQAsAFsAbABvAG8AawB1AHAAMQBdACwAWwBsAG8AbwBrAHUAcAAyAF0ALABbAGwAbwBvAGsAdQBwADMAXQAsAFsAbABvAG8AawB1AHAANABdACwAWwBsAG8AbwBrAHUAcAA1AF0ALABbAGwAbwBvAGsAdQBwADYAXQAsAFsAbABvAG8AawB1AHAANwBdACwAWwBsAG8AbwBrAHUAcAA4AF0ALABbAGwAbwBvAGsAdQBwADkAXQAsAFsAbABvAG8AawB1AHAAMQAwAF0ALABcAG4ATABFAFQAKABcAG4AXwBzACwAIABcACIAJQBeACYAJgBAAFwAIgAsACAAXABuAGwAbwBvAGsAdQBwAFYAYQBsAHUAZQAsACAAbABvAG8AawB1AHAAMQAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAMgAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAMwAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAANAAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAANQAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAANgAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAANwAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAOAAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAOQAgACYAIABfAHMAIAAmACAAbABvAG8AawB1AHAAMQAwACwAXABuAGwAZQB2AGUAbABJAG4AZABlAHgALAAgAEkARgBFAFIAUgBPAFIAKABSAE8AVwBTACgAVABFAFgAVABTAFAATABJAFQAKABsAG8AbwBrAHUAcABWAGEAbAB1AGUALAAgACwAIABfAHMALAAgAFQAUgBVAEUAKAApACkAKQAsACAAMAApACAAKwAgADEALAAgAFwAbgBsAG8AbwBrAHUAcABBAHIAcgBhAHkALAAgAEIAWQBSAE8AVwAoAEUAWABQAEEATgBEACgAQwBIAE8ATwBTAEUAQwBPAEwAUwAoAHIAYQBuAGcAZQAsACAAUwBFAFEAVQBFAE4AQwBFACgAMQAsACAAbABlAHYAZQBsAEkAbgBkAGUAeAAgAC0AIAAxACkAKQAsACAALAAgADEAMAAsACAAXAAiAFwAIgApACwAIABMAEEATQBCAEQAQQAoAHIAbwB3ACwAIABUAEUAWABUAEoATwBJAE4AKABfAHMALAAgAEYAQQBMAFMARQAsACAAcgBvAHcAKQApACkALABcAG4AcgBlAHQAdQByAG4AUgBhAG4AZwBlACwAIABJAE4ARABFAFgAKAByAGEAbgBnAGUALAAgADAALAAgAGwAZQB2AGUAbABJAG4AZABlAHgAKQAsACAAXABuAHIAZQBzAHUAbAB0ACwAIABJAEYAKABJAFMATwBNAEkAVABUAEUARAAoAGwAbwBvAGsAdQBwADEAKQAgACoAIABsAGUAdgBlAGwASQBuAGQAZQB4ACAAPQAgADEALAAgAHIAZQB0AHUAcgBuAFIAYQBuAGcAZQAsACAAWABMAE8ATwBLAFUAUAAoAGwAbwBvAGsAdQBwAFYAYQBsAHUAZQAsACAAbABvAG8AawB1AHAAQQByAHIAYQB5ACwAIAByAGUAdAB1AHIAbgBSAGEAbgBnAGUAKQA6AFgATABPAE8ASwBVAFAAKABsAG8AbwBrAHUAcABWAGEAbAB1AGUALAAgAGwAbwBvAGsAdQBwAEEAcgByAGEAeQAsACAAcgBlAHQAdQByAG4AUgBhAG4AZwBlACwAIAAsACAALAAgAC0AMQApACkALABcAG4AcgBlAHMAdQBsAHQAKQApADsAXABuAFwAbgAvAC8AIABNAGEAcgBrACAAUAByAG8AYwB0AG8AcgAgAEQARABMAFMAbwByAHQAZQByACAAZgB1AG4AYwB0AGkAbwBuAFwAbgBcAG4ARABEAEwAUwBvAHIAdABlAHIAPQBMAEEATQBCAEQAQQAoAFIAYQBuAGcAZQAsAFsAUwBvAHIAdABPAHIAZABlAHIAXQAsAFMATwBSAFQAKABSAGEAbgBnAGUALAAgAFMARQBRAFUARQBOAEMARQAoACwAIABDAE8ATABVAE0ATgBTACgAUgBhAG4AZwBlACkAKQAsACAAUwBvAHIAdABPAHIAZABlAHIAKQApADsAXABuAFwAbgAvAC8AIABEAG8AdQBiAGwAZQAgAFgATABPAE8ASwBVAFAAXABuAFwAbgBfAGYARABYAD0ATABBAE0AQgBEAEEAKAB2AGwAbwBvAGsAdQBwAF8AdgBhAGwAdQBlACwAdgBsAG8AbwBrAHUAcABfAGEAcgByAGEAeQAsAGgAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALABoAGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABbAGkAZgBfAG4AbwB0AF8AZgBvAHUAbgBkAF0ALABbAHYAbQBhAHQAYwBoAF8AbQBvAGQAZQBdACwAWwB2AHMAZQBhAHIAYwBoAF8AbQBvAGQAZQBdACwAWwBoAG0AYQB0AGMAaABfAG0AbwBkAGUAXQAsAFsAaABzAGUAYQByAGMAaABfAG0AbwBkAGUAXQAsACAASQBGAEUAUgBSAE8AUgAoACAASQBOAEQARQBYACgAcgBlAHQAdQByAG4AXwBhAHIAcgBhAHkALABYAE0AQQBUAEMASAAoAHYAbABvAG8AawB1AHAAXwB2AGEAbAB1AGUALAB2AGwAbwBvAGsAdQBwAF8AYQByAHIAYQB5ACwAdgBtAGEAdABjAGgAXwBtAG8AZABlACwAdgBzAGUAYQByAGMAaABfAG0AbwBkAGUAKQAsAFgATQBBAFQAQwBIACgAaABsAG8AbwBrAHUAcABfAHYAYQBsAHUAZQAsAGgAbABvAG8AawB1AHAAXwBhAHIAcgBhAHkALABoAG0AYQB0AGMAaABfAG0AbwBkAGUALABoAHMAZQBhAHIAYwBoAF8AbQBvAGQAZQApACkALAAgAEkARgAoAEkAUwBPAE0AbABUAFQARQBEACgAaQBmAF8AbgBvAHQAXwBmAG8AdQBuAGQAKQAsAE4AQQAoACkALABpAGYAXwBuAG8AdABfAGYAbwB1AG4AZAApACkAKQA7AFwAbgBcAG4ALwAvACAAUQB1AGEAcgB0AGUAcgAgAGYAcgBvAG0AIABNAG8AbgB0AGgAIABBAGIAYgByAGUAdgBpAGEAdABpAG8AbgBcAG4AXABuAF8AZgBRAD0ATABBAE0AQgBEAEEAKAB4ACwAUgBPAFUATgBEAFUAUAAoAE0ATwBOAFQASAAoADEAJgB4ACkALwAzACwAMAApACkAOwAiAH0AXQAsACIAcAByAG8AagBlAGMAdABOAGEAbQBlAHMAIgA6AFsAIgBfAGYASQBuAGQAZQB4ACIALAAiAF8AZgBTAFUAUABFAFIAWABMAE8ATwBLAFUAUAAiACwAIgBfAGYASQBuAHQAZQByAHAAIgAsACIAXwBmAEMAaABhAHIAQwBvAHUAbgB0ACIALAAiAF8AZgBEAE4AIgAsACIAXwBmAFUAUAAiACwAIgBfAGYAQgBDAEEAUwBUACIALAAiAEQARABMACIALAAiAEQARABMAFMAbwByAHQAZQByACIALAAiAF8AZgBEAFgAIgAsACIAXwBmAFEAIgBdACwAIgBsAG8AYwBhAGwAZQAiADoAewAiAGwAaQBzAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgByAG8AdwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgA7ACIALAAiAGMAbwBsAHUAbQBuAFMAZQBwAGEAcgBhAHQAbwByACIAOgAiACwAIgAsACIAdABoAG8AdQBzAGEAbgBkAHMAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBQAG8AcwBpAHQAaQBvAG4AcwAiADoAWwAzAF0ALAAiAGQAZQBjAGkAbQBhAGwAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALgAiACwAIgBkAGEAdABlAE8AcgBkAGUAcgAiADoAIgBEAE0AWQAiACwAIgBjAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwAIgA6ACIAJAAiACwAIgBpAHMAQwB1AHIAcgBlAG4AYwB5AFMAeQBtAGIAbwBsAEwAZQBhAGQAIgA6AHQAcgB1AGUALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwBlAHAAQgB5AFMAcABhAGMAZQAiADoAZgBhAGwAcwBlACwAIgByAG8AdwBMAGUAdAB0AGUAcgAiADoAIgBSACIALAAiAGMAbwBsAHUAbQBuAEwAZQB0AHQAZQByACIAOgAiAEMAIgAsACIAcgBjAEwAZQBmAHQAQgByAGEAYwBrAGUAdAAiADoAIgBbACIALAAiAHIAYwBSAGkAZwBoAHQAQgByAGEAYwBrAGUAdAAiADoAIgBdACIALAAiAHMAdABhAHQAZQBtAGUAbgB0AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAbABvAGMAYQBsAGUATgBhAG0AZQAiADoAIgBlAG4ALQB1AHMAIgB9AH0A</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5714F15D-BBBC-4CEE-B2FC-197F7FBAB617}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>